<commit_message>
Se registro nuevo caso de uso que se implementara y que hace referencia al alquiler de angares
</commit_message>
<xml_diff>
--- a/Gestión/Priorización.xlsx
+++ b/Gestión/Priorización.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="18915" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="18915" windowHeight="8505"/>
   </bookViews>
   <sheets>
     <sheet name="CUS" sheetId="1" r:id="rId1"/>
@@ -449,14 +449,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -757,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B4:C54"/>
+  <dimension ref="B2:C52"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1"/>
@@ -769,309 +769,317 @@
     <col min="3" max="3" width="49.28515625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:3" ht="15" customHeight="1">
+      <c r="B2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15" customHeight="1">
+      <c r="B3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="4" spans="2:3" ht="15" customHeight="1">
-      <c r="B4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>0</v>
+      <c r="B4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15" customHeight="1">
       <c r="B5" s="8" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15" customHeight="1">
       <c r="B6" s="8" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>49</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15" customHeight="1">
       <c r="B7" s="8" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15" customHeight="1">
       <c r="B8" s="8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15" customHeight="1">
       <c r="B9" s="8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="15" customHeight="1">
       <c r="B10" s="8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15" customHeight="1">
       <c r="B11" s="8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="15" customHeight="1">
       <c r="B12" s="8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="15" customHeight="1">
       <c r="B13" s="8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="15" customHeight="1">
       <c r="B14" s="8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="15" customHeight="1">
       <c r="B15" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="15" customHeight="1">
       <c r="B16" s="8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="15" customHeight="1">
       <c r="B17" s="8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="15" customHeight="1">
       <c r="B18" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="15" customHeight="1">
       <c r="B19" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="15" customHeight="1">
       <c r="B20" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="15" customHeight="1">
       <c r="B21" s="8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="15" customHeight="1">
       <c r="B22" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="15" customHeight="1">
       <c r="B23" s="8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="15" customHeight="1">
       <c r="B24" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="15" customHeight="1">
       <c r="B25" s="8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="15" customHeight="1">
       <c r="B26" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="15" customHeight="1">
       <c r="B27" s="8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="15" customHeight="1">
       <c r="B28" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="15" customHeight="1">
       <c r="B29" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="15" customHeight="1">
       <c r="B30" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="15" customHeight="1">
       <c r="B31" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="15" customHeight="1">
       <c r="B32" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="15" customHeight="1">
       <c r="B33" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="15" customHeight="1">
       <c r="B34" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="15" customHeight="1">
       <c r="B35" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="15" customHeight="1">
       <c r="B36" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="15" customHeight="1">
       <c r="B37" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="2:3" ht="15" customHeight="1">
       <c r="B38" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="15" customHeight="1">
       <c r="B39" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="2:3" ht="15" customHeight="1">
-      <c r="B40" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>81</v>
-      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="5"/>
     </row>
     <row r="41" spans="2:3" ht="15" customHeight="1">
-      <c r="B41" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>89</v>
-      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="5"/>
     </row>
     <row r="42" spans="2:3" ht="15" customHeight="1">
       <c r="B42" s="3"/>
@@ -1106,24 +1114,16 @@
       <c r="C49" s="5"/>
     </row>
     <row r="50" spans="2:3" ht="15" customHeight="1">
-      <c r="B50" s="3"/>
-      <c r="C50" s="5"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="2"/>
     </row>
     <row r="51" spans="2:3" ht="15" customHeight="1">
-      <c r="B51" s="3"/>
-      <c r="C51" s="5"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="2"/>
     </row>
     <row r="52" spans="2:3" ht="15" customHeight="1">
       <c r="B52" s="1"/>
       <c r="C52" s="2"/>
-    </row>
-    <row r="53" spans="2:3" ht="15" customHeight="1">
-      <c r="B53" s="1"/>
-      <c r="C53" s="2"/>
-    </row>
-    <row r="54" spans="2:3" ht="15" customHeight="1">
-      <c r="B54" s="1"/>
-      <c r="C54" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1135,9 +1135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AM161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B126" sqref="B126"/>
-    </sheetView>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -12518,10 +12516,10 @@
       <c r="B84" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C84" s="23" t="s">
+      <c r="C84" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D84" s="23"/>
+      <c r="D84" s="21"/>
     </row>
     <row r="85" spans="1:4" ht="15" customHeight="1">
       <c r="A85" s="8" t="s">
@@ -13005,12 +13003,12 @@
       <c r="D121" s="22"/>
     </row>
     <row r="123" spans="1:4" ht="15" customHeight="1">
-      <c r="A123" s="21" t="s">
+      <c r="A123" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="B123" s="21"/>
-      <c r="C123" s="21"/>
-      <c r="D123" s="21"/>
+      <c r="B123" s="23"/>
+      <c r="C123" s="23"/>
+      <c r="D123" s="23"/>
     </row>
     <row r="124" spans="1:4" ht="15" customHeight="1">
       <c r="A124" s="14" t="s">
@@ -13473,26 +13471,12 @@
     <sortCondition descending="1" ref="C125:C161"/>
   </sortState>
   <mergeCells count="39">
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="A123:D123"/>
+    <mergeCell ref="C117:D117"/>
+    <mergeCell ref="C118:D118"/>
+    <mergeCell ref="C119:D119"/>
+    <mergeCell ref="C120:D120"/>
+    <mergeCell ref="C121:D121"/>
     <mergeCell ref="C104:D104"/>
     <mergeCell ref="C116:D116"/>
     <mergeCell ref="C105:D105"/>
@@ -13506,12 +13490,26 @@
     <mergeCell ref="C113:D113"/>
     <mergeCell ref="C114:D114"/>
     <mergeCell ref="C115:D115"/>
-    <mergeCell ref="A123:D123"/>
-    <mergeCell ref="C117:D117"/>
-    <mergeCell ref="C118:D118"/>
-    <mergeCell ref="C119:D119"/>
-    <mergeCell ref="C120:D120"/>
-    <mergeCell ref="C121:D121"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C88:D88"/>
   </mergeCells>
   <pageMargins left="0.11811023622047245" right="0.51181102362204722" top="0.15748031496062992" bottom="0.15748031496062992" header="0.11811023622047245" footer="0.15748031496062992"/>
   <pageSetup scale="50" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>